<commit_message>
Minor updates and refactoring
Utilities.js – refactor from TokenCollision(x1, y1, x2, y2) to TokenCollision(token1, token2)

Tokens.js – removed .currentTile
</commit_message>
<xml_diff>
--- a/06_js_game.xlsx
+++ b/06_js_game.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbayes/GitHub/06_js_game/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paganbear/Development/GitHub/06_js_game/06_js_game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848AF2C2-C189-AB43-925B-0E570AC3FD19}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6497210-159D-C140-980D-B7BA0BE0503C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="17200" windowHeight="16080" xr2:uid="{71FD1CF9-53E8-634D-8FF4-141EDE15809D}"/>
   </bookViews>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
   <si>
     <t>index.js</t>
   </si>
@@ -176,9 +171,6 @@
     <t>Utilities.UpdateGameTable()</t>
   </si>
   <si>
-    <t>Utilities.TokenCollision(x1, y1, x2, y2)</t>
-  </si>
-  <si>
     <t>Utilities.SetCoords()</t>
   </si>
   <si>
@@ -206,9 +198,6 @@
     <t>.removeClass()</t>
   </si>
   <si>
-    <t>.addClass()</t>
-  </si>
-  <si>
     <t>.text(str)</t>
   </si>
   <si>
@@ -228,13 +217,31 @@
   </si>
   <si>
     <t>obj.hasOwnProperty(key)</t>
+  </si>
+  <si>
+    <t>.addClass(arr)</t>
+  </si>
+  <si>
+    <t>Utilities.TokenCollision(token1, token2)</t>
+  </si>
+  <si>
+    <t>assignColor()</t>
+  </si>
+  <si>
+    <t>clearToken()</t>
+  </si>
+  <si>
+    <t>fillToken()</t>
+  </si>
+  <si>
+    <t>pickRandomWeapon()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -259,6 +266,11 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Courier New"/>
       <family val="1"/>
     </font>
@@ -294,12 +306,12 @@
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,11 +626,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BE388F-BEDE-E74D-B2E2-06F9B884358A}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -638,7 +650,7 @@
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -656,365 +668,385 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D4" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D5" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" s="4" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D21" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D23" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D26" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D27" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D29" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D30" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D31" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D32" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D33" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D37" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D38" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D39" s="4" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D42" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D40" s="4" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D41" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D42" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>31</v>
+      <c r="D45" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D46" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D47" s="1" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D48" s="1" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D49" s="3" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D50" s="1" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D51" s="3" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D55" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D56" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D57" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D52" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D53" s="3" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D58" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D59" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D60" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D61" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D54" s="3" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D62" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D63" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D64" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D65" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D66" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D55" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D56" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D57" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D58" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D59" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D60" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D61" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D62" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D63" s="7" t="s">
-        <v>54</v>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D67" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>